<commit_message>
first push for control
</commit_message>
<xml_diff>
--- a/mini-projet-trey/input-data/trey_power_network.xlsx
+++ b/mini-projet-trey/input-data/trey_power_network.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eistore2\iese\institut\Laboratoires\Labo_MRB\RHT\Labo\teams_lab_pack_2024-2025\mini-projet-trey\input-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\matthjoye\github\rhtlab_MIB\mini-projet-trey\input-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD5684B-AA1E-4BE0-9588-B2D026B68503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE473614-C12B-4AEE-9799-813433ECF547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -443,10 +443,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+    <cellStyle name="Insatisfaisant" xfId="3" builtinId="27"/>
+    <cellStyle name="Neutre" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -462,7 +462,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -764,13 +764,13 @@
       <selection activeCell="C2" sqref="C2:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
-    <col min="2" max="2" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -790,7 +790,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -804,7 +804,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -818,7 +818,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -832,7 +832,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -846,7 +846,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -860,7 +860,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -874,7 +874,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -888,7 +888,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -902,7 +902,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -916,7 +916,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -930,7 +930,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -944,7 +944,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -958,7 +958,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -972,92 +972,92 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1072,22 +1072,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D466C24-507B-41DF-96AE-5E0A3D434556}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:I12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.36328125" customWidth="1"/>
-    <col min="7" max="7" width="15.54296875" customWidth="1"/>
-    <col min="11" max="11" width="10.36328125" customWidth="1"/>
-    <col min="12" max="12" width="15.6328125" customWidth="1"/>
-    <col min="13" max="13" width="16.36328125" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1156,8 +1156,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E2">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1170,8 +1173,11 @@
       <c r="D3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1184,9 +1190,12 @@
       <c r="D4">
         <v>3</v>
       </c>
+      <c r="E4">
+        <v>0.115</v>
+      </c>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1199,9 +1208,12 @@
       <c r="D5">
         <v>4</v>
       </c>
+      <c r="E5">
+        <v>0.08</v>
+      </c>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1214,8 +1226,11 @@
       <c r="D6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E6">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1228,8 +1243,11 @@
       <c r="D7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E7">
+        <v>0.13500000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1242,9 +1260,12 @@
       <c r="D8">
         <v>7</v>
       </c>
+      <c r="E8">
+        <v>0.1</v>
+      </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1257,9 +1278,12 @@
       <c r="D9">
         <v>8</v>
       </c>
+      <c r="E9">
+        <v>0.20499999999999999</v>
+      </c>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1272,8 +1296,11 @@
       <c r="D10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E10">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1286,8 +1313,11 @@
       <c r="D11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E11">
+        <v>0.255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1300,103 +1330,106 @@
       <c r="D12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E12">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1414,12 +1447,12 @@
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1451,157 +1484,157 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1619,17 +1652,17 @@
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
-    <col min="15" max="15" width="14.08984375" customWidth="1"/>
-    <col min="17" max="17" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.453125" customWidth="1"/>
-    <col min="24" max="24" width="19.453125" customWidth="1"/>
-    <col min="26" max="26" width="18.6328125" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.109375" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.44140625" customWidth="1"/>
+    <col min="24" max="24" width="19.44140625" customWidth="1"/>
+    <col min="26" max="26" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -1721,7 +1754,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1756,152 +1789,152 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1919,15 +1952,15 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" style="8"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="8" width="16.36328125" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="8"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1968,7 +2001,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1989,153 +2022,153 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2154,17 +2187,17 @@
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
-    <col min="2" max="7" width="10.6328125" customWidth="1"/>
-    <col min="8" max="8" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="10.6328125" customWidth="1"/>
-    <col min="12" max="12" width="17.08984375" customWidth="1"/>
-    <col min="13" max="24" width="10.6328125" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" customWidth="1"/>
+    <col min="13" max="24" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2205,157 +2238,157 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2371,19 +2404,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB91AA0C-6E10-4C2C-B831-A2E20673E5F8}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
-    <col min="7" max="7" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2421,7 +2454,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2432,7 +2465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2443,7 +2476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2454,7 +2487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2465,7 +2498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2476,7 +2509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2487,7 +2520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2498,7 +2531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2509,7 +2542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2520,7 +2553,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2531,7 +2564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2542,7 +2575,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2553,97 +2586,97 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>

</xml_diff>